<commit_message>
Lisää suunniteltu määrä exceliin ja korjaa testit
</commit_message>
<xml_diff>
--- a/test/resurssit/excel/Paikkausehdotukset.xlsx
+++ b/test/resurssit/excel/Paikkausehdotukset.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
   <si>
     <t xml:space="preserve">Paikkausehdotukset 2021</t>
   </si>
@@ -65,6 +65,9 @@
     <t xml:space="preserve">Määrä</t>
   </si>
   <si>
+    <t xml:space="preserve">Yksikkö</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kustannusarvio</t>
   </si>
   <si>
@@ -86,9 +89,6 @@
     <t xml:space="preserve">Myrskyläntien tärinätalon kohta</t>
   </si>
   <si>
-    <t xml:space="preserve">Konetiivistetty reikävaluasfalttipaikkaus (REPA)</t>
-  </si>
-  <si>
     <t xml:space="preserve">t</t>
   </si>
   <si>
@@ -104,9 +104,6 @@
     <t xml:space="preserve">Mt 280 Somerontien hienojyrsintä</t>
   </si>
   <si>
-    <t xml:space="preserve">AB-paikkaus levittäjällä (POT-ilmoitus tehdään)</t>
-  </si>
-  <si>
     <t xml:space="preserve">m2</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
   </si>
   <si>
     <t xml:space="preserve">Paikkausmenetelmät</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yksikkö</t>
   </si>
   <si>
     <t xml:space="preserve">AB-paikkaus levittäjällä </t>
@@ -212,6 +206,9 @@
   </si>
   <si>
     <t xml:space="preserve">KT-valuasfalttipaikkaus (KTVA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Konetiivistetty reikävaluasfalttipaikkaus (REPA)</t>
   </si>
   <si>
     <t xml:space="preserve">Sirotepuhalluspaikkaus (SIPU)</t>
@@ -438,7 +435,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -569,10 +566,6 @@
     </xf>
     <xf numFmtId="168" fontId="11" fillId="2" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -602,13 +595,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O1048576"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M29" activeCellId="0" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.25"/>
@@ -619,12 +612,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="47.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="45.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="45.4"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -640,10 +633,11 @@
       <c r="K1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="4"/>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N1" s="2"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -657,10 +651,11 @@
       <c r="K2" s="1"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N2" s="2"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -674,10 +669,11 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="4"/>
-    </row>
-    <row r="4" s="13" customFormat="true" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N3" s="2"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4" s="13" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -717,19 +713,22 @@
       <c r="M4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P4" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="n">
         <v>1</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="16" t="n">
         <v>11746</v>
@@ -741,28 +740,31 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O5" s="20"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M5" s="17" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P5" s="20"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="n">
         <v>2</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="21" t="n">
         <v>1605</v>
@@ -776,17 +778,20 @@
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="N6" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O6" s="20"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O6" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P6" s="20"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="n">
         <v>3</v>
       </c>
@@ -803,19 +808,22 @@
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
       <c r="L7" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="17" t="n">
+        <v>10</v>
+      </c>
+      <c r="N7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="N7" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O7" s="23" t="s">
+      <c r="O7" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P7" s="23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="n">
         <v>4</v>
       </c>
@@ -834,24 +842,27 @@
       <c r="J8" s="25"/>
       <c r="K8" s="25"/>
       <c r="L8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="17" t="n">
+        <v>100</v>
+      </c>
+      <c r="N8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="O8" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O8" s="23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="n">
         <v>5</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="21" t="n">
         <v>2805</v>
@@ -865,18 +876,19 @@
       <c r="J9" s="25"/>
       <c r="K9" s="25"/>
       <c r="L9" s="17"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O9" s="20"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M9" s="17"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P9" s="20"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="n">
         <v>6</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="26" t="n">
         <v>11307</v>
@@ -890,18 +902,19 @@
       <c r="J10" s="25"/>
       <c r="K10" s="14"/>
       <c r="L10" s="17"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O10" s="20"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M10" s="17"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P10" s="20"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="n">
         <v>7</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="16" t="n">
         <v>11875</v>
@@ -915,18 +928,19 @@
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
       <c r="L11" s="17"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O11" s="20"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M11" s="17"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P11" s="20"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="n">
         <v>9</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="28" t="n">
         <v>25</v>
@@ -940,20 +954,21 @@
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
       <c r="L12" s="17"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O12" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M12" s="17"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P12" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="n">
         <v>10</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="28" t="n">
         <v>104</v>
@@ -967,20 +982,21 @@
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
       <c r="L13" s="17"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O13" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M13" s="17"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P13" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="n">
         <v>11</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="28" t="n">
         <v>1015</v>
@@ -994,18 +1010,19 @@
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
       <c r="L14" s="17"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O14" s="20"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M14" s="17"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P14" s="20"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="14" t="n">
         <v>19</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="16" t="n">
         <v>1131</v>
@@ -1019,20 +1036,21 @@
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
       <c r="L15" s="17"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O15" s="20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M15" s="17"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P15" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="n">
         <v>20</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="21" t="n">
         <v>21530</v>
@@ -1046,20 +1064,21 @@
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
       <c r="L16" s="17"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O16" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M16" s="17"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P16" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="n">
         <v>33</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="26" t="n">
         <v>11289</v>
@@ -1085,20 +1104,21 @@
       <c r="J17" s="25"/>
       <c r="K17" s="25"/>
       <c r="L17" s="17"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O17" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M17" s="17"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P17" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="n">
         <v>35</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="28" t="n">
         <v>11187</v>
@@ -1112,20 +1132,21 @@
       <c r="J18" s="25"/>
       <c r="K18" s="25"/>
       <c r="L18" s="17"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O18" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M18" s="17"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P18" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="n">
         <v>36</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="28" t="n">
         <v>11241</v>
@@ -1139,18 +1160,19 @@
       <c r="J19" s="25"/>
       <c r="K19" s="25"/>
       <c r="L19" s="17"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O19" s="20"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M19" s="17"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P19" s="20"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="n">
         <v>41</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="21" t="n">
         <v>11721</v>
@@ -1168,23 +1190,24 @@
       <c r="J20" s="25"/>
       <c r="K20" s="25"/>
       <c r="L20" s="17"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="O20" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M20" s="17"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P20" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="n">
         <v>51</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="25"/>
@@ -1195,35 +1218,35 @@
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
       <c r="L21" s="17"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="32" t="n">
+      <c r="M21" s="17"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="32" t="n">
         <v>0</v>
       </c>
-      <c r="O21" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="33"/>
+      <c r="P21" s="20" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="34"/>
+      <c r="B28" s="33"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K2"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M5:M21" type="list">
+  <dataValidations count="3">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N5:N21" type="list">
       <formula1>Lähtötiedot!$B$2:$B$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L5:L21" type="list">
+      <formula1>Lähtötiedot!$A$2:$A$17</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M5:M21" type="none">
       <formula1>Lähtötiedot!$A$2:$A$17</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1249,106 +1272,106 @@
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.328125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="50.20703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="34" t="s">
         <v>51</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="35" t="s">
-        <v>53</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B4" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="34" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="35" t="s">
-        <v>21</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="34" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="35" t="s">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="34" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="35" t="s">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="34" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="35" t="s">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="34" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="35" t="s">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="35" t="s">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="35" t="s">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="34" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35" t="s">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="35" t="s">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="34" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="35" t="s">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="35" t="s">
-        <v>67</v>
-      </c>
-    </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="35" t="s">
-        <v>18</v>
+      <c r="A17" s="34" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>